<commit_message>
Login and Signin Demo
</commit_message>
<xml_diff>
--- a/SoftwareEngineeringStuff/BurnDownChart.xlsx
+++ b/SoftwareEngineeringStuff/BurnDownChart.xlsx
@@ -1173,13 +1173,10 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>61</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1194,11 +1191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="259441032"/>
-        <c:axId val="257849016"/>
+        <c:axId val="275286256"/>
+        <c:axId val="275286648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="259441032"/>
+        <c:axId val="275286256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,12 +1308,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257849016"/>
+        <c:crossAx val="275286648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257849016"/>
+        <c:axId val="275286648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,7 +1431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259441032"/>
+        <c:crossAx val="275286256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2372,7 +2369,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2391,7 @@
       </c>
       <c r="B2">
         <f>SUM(B3:B16)</f>
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2452,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2468,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2484,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2516,7 +2513,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2648,7 @@
         <v>42</v>
       </c>
       <c r="D9">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2665,7 +2662,7 @@
         <v>41</v>
       </c>
       <c r="D10">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2677,9 +2674,6 @@
       </c>
       <c r="C11">
         <v>40</v>
-      </c>
-      <c r="D11">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Massive change and modifications
</commit_message>
<xml_diff>
--- a/SoftwareEngineeringStuff/BurnDownChart.xlsx
+++ b/SoftwareEngineeringStuff/BurnDownChart.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kwangju\Documents\GitHub\ProjectAppStuff\ProjectAppStuff\SoftwareEngineeringStuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kwangju\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId2"/>
+    <sheet name="Chart" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Total</t>
   </si>
@@ -103,6 +104,33 @@
   </si>
   <si>
     <t>HTML stuff</t>
+  </si>
+  <si>
+    <t>Plan and Design Database</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Make the proper results..</t>
+  </si>
+  <si>
+    <t>Forum class</t>
+  </si>
+  <si>
+    <t>Edit and config app class</t>
+  </si>
+  <si>
+    <t>Login/LoginHandlng</t>
+  </si>
+  <si>
+    <t>Search bar</t>
+  </si>
+  <si>
+    <t>Servelets</t>
+  </si>
+  <si>
+    <t>Get info…</t>
   </si>
 </sst>
 </file>
@@ -519,154 +547,154 @@
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>48</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>47</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>47</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>47</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>46</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>46</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>46</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>35</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>31</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>27</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>24</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>22</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>21</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>20</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,200 +932,194 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$C$2:$C$65</c:f>
+              <c:f>Chart!$C$2:$C$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>52</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>39</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>38</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>33</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>29</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>22</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>21</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>19</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="63">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1337,6 +1359,33 @@
                 <c:pt idx="12">
                   <c:v>51</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>38</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1350,11 +1399,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251564632"/>
-        <c:axId val="251565416"/>
+        <c:axId val="249258560"/>
+        <c:axId val="249260520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251564632"/>
+        <c:axId val="249258560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,12 +1516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251565416"/>
+        <c:crossAx val="249260520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251565416"/>
+        <c:axId val="249260520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,7 +1639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251564632"/>
+        <c:crossAx val="249258560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2699,10 +2748,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <f>SUM(B2:B9)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2872,7 @@
         <v>49</v>
       </c>
       <c r="C2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>49</v>
@@ -2746,7 +2886,7 @@
         <v>49</v>
       </c>
       <c r="C3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>49</v>
@@ -2764,7 +2904,7 @@
         <v>51</v>
       </c>
       <c r="C4">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>49</v>
@@ -2778,7 +2918,7 @@
         <v>56</v>
       </c>
       <c r="C5">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>49</v>
@@ -2792,7 +2932,7 @@
         <v>64</v>
       </c>
       <c r="C6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>49</v>
@@ -2806,7 +2946,7 @@
         <v>65</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>65</v>
@@ -2820,7 +2960,7 @@
         <v>64</v>
       </c>
       <c r="C8">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>64</v>
@@ -2834,7 +2974,7 @@
         <v>63</v>
       </c>
       <c r="C9">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>62</v>
@@ -2848,7 +2988,7 @@
         <v>62</v>
       </c>
       <c r="C10">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2862,7 +3002,7 @@
         <v>59</v>
       </c>
       <c r="C11">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>59</v>
@@ -2876,7 +3016,7 @@
         <v>57</v>
       </c>
       <c r="C12">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>58</v>
@@ -2890,7 +3030,7 @@
         <v>53</v>
       </c>
       <c r="C13">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <f>38+13</f>
@@ -2905,7 +3045,7 @@
         <v>51</v>
       </c>
       <c r="C14">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14">
         <f>51</f>
@@ -2920,6 +3060,9 @@
         <v>51</v>
       </c>
       <c r="C15">
+        <v>48</v>
+      </c>
+      <c r="D15">
         <v>50</v>
       </c>
     </row>
@@ -2928,186 +3071,210 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C18">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C20">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C23">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C24">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C26">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3115,10 +3282,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3126,10 +3293,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C34">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3137,10 +3304,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C35">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,10 +3315,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C36">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3159,10 +3326,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C37">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3170,10 +3337,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C38">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,10 +3348,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C39">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3192,10 +3359,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C40">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,10 +3370,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C41">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3214,10 +3381,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3225,10 +3392,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C43">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3236,10 +3403,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C44">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3247,10 +3414,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C45">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3258,10 +3425,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C46">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3269,10 +3436,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3280,10 +3447,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3291,10 +3458,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,10 +3469,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3313,10 +3480,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C51">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3324,10 +3491,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3335,10 +3502,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3346,10 +3513,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C54">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3357,10 +3524,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C55">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3368,10 +3535,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C56">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3379,10 +3546,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3390,10 +3557,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C58">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,10 +3568,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3412,10 +3579,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3423,10 +3590,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3434,10 +3601,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3445,10 +3612,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,10 +3623,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3634,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>

</xml_diff>